<commit_message>
seed walks Table added
</commit_message>
<xml_diff>
--- a/plan/Database Schema.xlsx
+++ b/plan/Database Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JacobField\Desktop\Pawsome Walks\pawsome-walks\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681C99FE-28E3-477E-BDCE-916E421F278C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A62C723-F723-4451-807C-A4A1475C466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{792DDB20-CFC8-4D18-9397-042A1C0BB0C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{792DDB20-CFC8-4D18-9397-042A1C0BB0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="153">
   <si>
     <t>ownerId</t>
   </si>
@@ -104,9 +104,6 @@
     <t>walkType</t>
   </si>
   <si>
-    <t>offLeadArea</t>
-  </si>
-  <si>
     <t>paths</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>FLOAT</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>receiverDogId</t>
   </si>
   <si>
@@ -449,9 +443,6 @@
     <t>Retrieves all comments by walkId</t>
   </si>
   <si>
-    <t>commentId</t>
-  </si>
-  <si>
     <t>/walkComments/:commentId</t>
   </si>
   <si>
@@ -489,6 +480,21 @@
   </si>
   <si>
     <t>retrieves all friend requests a specific dog has received</t>
+  </si>
+  <si>
+    <t>free/paid/none</t>
+  </si>
+  <si>
+    <t>dogPalRequestId</t>
+  </si>
+  <si>
+    <t>walkCommentId</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>offLeadAreas</t>
   </si>
 </sst>
 </file>
@@ -713,30 +719,6 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -770,28 +752,10 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -818,6 +782,12 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -827,9 +797,6 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -839,7 +806,46 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1178,98 +1184,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633C59CC-267A-4027-B294-767BC073E2ED}">
   <dimension ref="B2:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="16"/>
-    <col min="2" max="2" width="14.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" style="16" customWidth="1"/>
-    <col min="10" max="10" width="16" style="16" customWidth="1"/>
-    <col min="11" max="11" width="28.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" style="16" customWidth="1"/>
-    <col min="13" max="13" width="36.21875" style="16" customWidth="1"/>
-    <col min="14" max="14" width="12.21875" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="8.88671875" style="8"/>
+    <col min="2" max="2" width="14.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="16" style="8" customWidth="1"/>
+    <col min="11" max="11" width="28.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" style="8" customWidth="1"/>
+    <col min="13" max="13" width="36.21875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="12.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="B2" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="B5" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1286,7 +1292,7 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1303,256 +1309,256 @@
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C14" s="23"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="24" t="s">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="F15" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="J15" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="F15" s="25" t="s">
+      <c r="J18" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="J15" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="L16" s="40" t="s">
+      <c r="D19" s="44"/>
+      <c r="F19" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="42"/>
+      <c r="J19" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="M16" s="40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="K17" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="M17" s="40" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="M18" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="31"/>
-      <c r="F19" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="33"/>
-      <c r="J19" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="K19" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="L19" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="M19" s="43"/>
+      <c r="M19" s="31"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
+      <c r="B21" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="45"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
@@ -1577,25 +1583,25 @@
         <v>21</v>
       </c>
       <c r="I22" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.3">
@@ -1612,42 +1618,42 @@
         <v>15</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="C24" s="34" t="s">
-        <v>45</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1660,70 +1666,72 @@
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
+      <c r="O24" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="26" spans="2:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-      <c r="I26" s="48" t="s">
+      <c r="B26" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="I26" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="J27" s="49" t="s">
+      <c r="L27" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="K27" s="49" t="s">
+      <c r="M27" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="L27" s="49" t="s">
+      <c r="N27" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="M27" s="49" t="s">
+      <c r="O27" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="N27" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="O27" s="49" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="28" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1736,132 +1744,132 @@
         <v>14</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>61</v>
+        <v>40</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N28" s="1">
         <v>201</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="36" t="s">
-        <v>45</v>
-      </c>
       <c r="D29" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G29" s="3"/>
-      <c r="I29" s="17" t="s">
-        <v>61</v>
+      <c r="I29" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N29" s="1">
         <v>200</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I30" s="17" t="s">
-        <v>61</v>
+      <c r="I30" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="J30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="N30" s="1">
         <v>200</v>
       </c>
       <c r="O30" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="38"/>
+      <c r="I31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="9"/>
-      <c r="I31" s="17" t="s">
+      <c r="K31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="M31" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N31" s="1">
         <v>200</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>16</v>
@@ -1870,35 +1878,35 @@
         <v>0</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J32" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="K32" s="20" t="s">
+      <c r="J32" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="N32" s="12">
+        <v>201</v>
+      </c>
+      <c r="O32" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L32" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="M32" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="N32" s="20">
-        <v>201</v>
-      </c>
-      <c r="O32" s="20" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1911,514 +1919,510 @@
         <v>14</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I33" s="19" t="s">
+      <c r="I33" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J33" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="K33" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L33" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="M33" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="N33" s="20">
+      <c r="J33" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="N33" s="12">
         <v>200</v>
       </c>
-      <c r="O33" s="20" t="s">
-        <v>88</v>
+      <c r="O33" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="38" t="s">
-        <v>45</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="I34" s="19" t="s">
+      <c r="I34" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J34" s="20" t="s">
+      <c r="J34" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="M34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="N34" s="12">
+        <v>200</v>
+      </c>
+      <c r="O34" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="K34" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L34" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="M34" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="N34" s="20">
+    </row>
+    <row r="35" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N35" s="12">
         <v>200</v>
       </c>
-      <c r="O34" s="20" t="s">
+      <c r="O35" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I35" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="K35" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L35" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="M35" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="N35" s="20">
+    <row r="36" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I36" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="M36" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="N36" s="18">
+        <v>201</v>
+      </c>
+      <c r="O36" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I37" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="L37" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="M37" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="N37" s="18">
         <v>200</v>
       </c>
-      <c r="O35" s="20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I36" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="K36" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="L36" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="M36" s="27" t="s">
+      <c r="O37" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I38" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K38" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M38" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="N36" s="27">
+      <c r="N38" s="18">
+        <v>200</v>
+      </c>
+      <c r="O38" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I39" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="L39" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="M39" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N39" s="19">
         <v>201</v>
       </c>
-      <c r="O36" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I37" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="J37" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="K37" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="L37" s="27" t="s">
+      <c r="O39" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I40" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="L40" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="M37" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="N37" s="27">
+      <c r="M40" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="N40" s="19">
         <v>200</v>
       </c>
-      <c r="O37" s="27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I38" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="J38" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="K38" s="27" t="s">
+      <c r="O40" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I41" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="L38" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="M38" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="N38" s="27">
+      <c r="J41" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="L41" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="N41" s="19">
         <v>200</v>
       </c>
-      <c r="O38" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I39" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J39" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="K39" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="L39" s="29" t="s">
+      <c r="O41" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I42" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J42" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="L42" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="M42" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42" s="26">
+        <v>201</v>
+      </c>
+      <c r="O42" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="M39" s="29" t="s">
+    </row>
+    <row r="43" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I43" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="K43" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="L43" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M43" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="N43" s="26">
+        <v>200</v>
+      </c>
+      <c r="O43" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="I44" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J44" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K44" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="L44" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M44" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="N39" s="29">
-        <v>201</v>
-      </c>
-      <c r="O39" s="29" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J40" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="K40" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="L40" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="M40" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="N40" s="29">
+      <c r="N44" s="26">
         <v>200</v>
       </c>
-      <c r="O40" s="29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I41" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="J41" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="K41" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="L41" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="M41" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="N41" s="29">
-        <v>200</v>
-      </c>
-      <c r="O41" s="29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I42" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="J42" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="K42" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="L42" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="M42" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="N42" s="40">
-        <v>201</v>
-      </c>
-      <c r="O42" s="40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="I43" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="J43" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="K43" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="L43" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="M43" s="40" t="s">
-        <v>140</v>
-      </c>
-      <c r="N43" s="40">
-        <v>200</v>
-      </c>
-      <c r="O43" s="40" t="s">
+      <c r="O44" s="26" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="I44" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="J44" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="K44" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="L44" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="M44" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="N44" s="40">
-        <v>200</v>
-      </c>
-      <c r="O44" s="40" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="45" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="I45" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N45" s="2">
         <v>200</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="I46" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N46" s="2">
         <v>200</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="2:15" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I47" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N47" s="2">
         <v>201</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="I48" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="L48" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="L48" s="3" t="s">
-        <v>124</v>
-      </c>
       <c r="M48" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N48" s="3">
         <v>201</v>
       </c>
       <c r="O48" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="9:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="I49" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L49" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N49" s="3">
         <v>200</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="50" spans="9:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="I50" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K50" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L50" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N50" s="3">
         <v>200</v>
       </c>
       <c r="O50" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="9:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="I51" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K51" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="51" spans="9:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I51" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="K51" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="L51" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N51" s="4">
         <v>201</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="9:15" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="I52" s="37" t="s">
-        <v>35</v>
+      <c r="I52" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="N52" s="4">
         <v>200</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="9:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="I53" s="37" t="s">
-        <v>35</v>
+      <c r="I53" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N53" s="4">
         <v>200</v>
       </c>
       <c r="O53" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="I26:O26"/>
+    <mergeCell ref="B2:J4"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="F15:H15"/>
@@ -2426,7 +2430,11 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B21:O21"/>
     <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B2:J4"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="I26:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>